<commit_message>
work on dropdown box for user management
</commit_message>
<xml_diff>
--- a/Project_TimeLine_2021_4_Mar.xlsx
+++ b/Project_TimeLine_2021_4_Mar.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Murphy Tan\Desktop\lms\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94999089-617F-43A6-818C-8AFA5404845C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{482EF86A-2A1D-4C59-B27D-1E25D53D6ACB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{5A8E5395-CCD6-4F57-83A8-81B53FE4AFF6}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="36">
   <si>
     <t>S/N</t>
   </si>
@@ -875,7 +875,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -894,9 +894,7 @@
       <c r="F15" s="3">
         <v>44272</v>
       </c>
-      <c r="I15" s="4" t="s">
-        <v>31</v>
-      </c>
+      <c r="I15" s="4"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16">

</xml_diff>